<commit_message>
EPBDS-14582 Fix serialization and deserialization using MixIn
</commit_message>
<xml_diff>
--- a/ITEST/itest.WebService/openl-repository/EPBDS-9581/EPBDS-9581/Main.xlsx
+++ b/ITEST/itest.WebService/openl-repository/EPBDS-9581/EPBDS-9581/Main.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
   <si>
     <t>Datatype Customer</t>
   </si>
@@ -43,6 +43,9 @@
     <t>privateField</t>
   </si>
   <si>
+    <t>dob_s</t>
+  </si>
+  <si>
     <t>Datatype Customer2</t>
   </si>
   <si>
@@ -56,6 +59,9 @@
   </si>
   <si>
     <t>Method Customer proxyCustomer(Customer c)</t>
+  </si>
+  <si>
+    <t>c.dob_s = toString(c.dob, "yyyy MM dd - HH mm ss");</t>
   </si>
   <si>
     <t>return c;</t>
@@ -88,12 +94,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -106,16 +118,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -132,16 +144,16 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -161,6 +173,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -360,17 +373,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -398,10 +411,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -649,12 +662,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -941,7 +954,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -969,10 +982,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1223,15 +1236,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="8.85156" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5469" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.4844" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" style="1" customWidth="1"/>
     <col min="4" max="5" width="8.85156" style="1" customWidth="1"/>
     <col min="6" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
@@ -1307,8 +1320,12 @@
     </row>
     <row r="8" ht="13.55" customHeight="1">
       <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="B8" t="s" s="5">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s" s="5">
+        <v>10</v>
+      </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
@@ -1329,7 +1346,7 @@
     <row r="11" ht="13.55" customHeight="1">
       <c r="A11" s="2"/>
       <c r="B11" t="s" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="2"/>
@@ -1355,7 +1372,7 @@
         <v>4</v>
       </c>
       <c r="D13" t="s" s="5">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E13" s="2"/>
     </row>
@@ -1383,8 +1400,12 @@
     </row>
     <row r="16" ht="13.55" customHeight="1">
       <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="B16" t="s" s="5">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s" s="5">
+        <v>10</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
@@ -1412,7 +1433,7 @@
     <row r="20" ht="13.55" customHeight="1">
       <c r="A20" s="2"/>
       <c r="B20" t="s" s="5">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -1421,7 +1442,7 @@
     <row r="21" ht="13.55" customHeight="1">
       <c r="A21" s="2"/>
       <c r="B21" t="s" s="5">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1430,7 +1451,7 @@
     <row r="22" ht="13.55" customHeight="1">
       <c r="A22" s="2"/>
       <c r="B22" t="s" s="5">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1462,7 +1483,7 @@
     <row r="26" ht="13.55" customHeight="1">
       <c r="A26" s="2"/>
       <c r="B26" t="s" s="5">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1471,7 +1492,7 @@
     <row r="27" ht="13.55" customHeight="1">
       <c r="A27" s="2"/>
       <c r="B27" t="s" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1479,7 +1500,9 @@
     </row>
     <row r="28" ht="13.55" customHeight="1">
       <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
+      <c r="B28" t="s" s="5">
+        <v>17</v>
+      </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1493,9 +1516,7 @@
     </row>
     <row r="30" ht="13.55" customHeight="1">
       <c r="A30" s="2"/>
-      <c r="B30" t="s" s="5">
-        <v>16</v>
-      </c>
+      <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1503,7 +1524,7 @@
     <row r="31" ht="13.55" customHeight="1">
       <c r="A31" s="2"/>
       <c r="B31" t="s" s="5">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -1511,14 +1532,18 @@
     </row>
     <row r="32" ht="13.55" customHeight="1">
       <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
+      <c r="B32" t="s" s="5">
+        <v>16</v>
+      </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
     </row>
     <row r="33" ht="13.55" customHeight="1">
       <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
+      <c r="B33" t="s" s="5">
+        <v>17</v>
+      </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -1585,6 +1610,20 @@
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
+    </row>
+    <row r="43" ht="13.55" customHeight="1">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" ht="13.55" customHeight="1">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>